<commit_message>
Data Cleaniup Round 2
</commit_message>
<xml_diff>
--- a/Data/Cleaned Data.xlsx
+++ b/Data/Cleaned Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="24810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="24810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -692,7 +692,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -838,7 +838,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="ANCLAS,REZONES Y SUS PARTES,DE FUNDICION,DE HIERRO O DE ACERO" xfId="1"/>
+    <cellStyle name="ANCLAS,REZONES Y SUS PARTES,DE FUNDICION,DE HIERRO O DE ACERO" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1150,11 +1150,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219:C219"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>